<commit_message>
Correct some column translations
</commit_message>
<xml_diff>
--- a/tables/column_name_translations/AT_column_name_translation.xlsx
+++ b/tables/column_name_translations/AT_column_name_translation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC853EED-90BA-49C6-AC42-33CDC05C786D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BC61BA-3EBD-4661-81F1-5514CEABA980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>field_id</t>
   </si>
@@ -219,17 +219,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -530,7 +524,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F9" sqref="F9"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,31 +586,31 @@
       <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="19" t="s">
         <v>47</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -642,15 +636,9 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
         <v>37</v>
       </c>
@@ -685,31 +673,31 @@
       <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="9" t="s">
         <v>38</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="19" t="s">
         <v>43</v>
       </c>
       <c r="N4" s="4"/>
@@ -729,34 +717,34 @@
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="I5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="J5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="14" t="s">
         <v>39</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="25" t="s">
+      <c r="M5" s="19" t="s">
         <v>44</v>
       </c>
       <c r="N5" s="4"/>
@@ -894,31 +882,25 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="I11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="J11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="19" t="s">
         <v>14</v>
       </c>
       <c r="L11" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="25"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -930,28 +912,34 @@
       <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="22" t="s">
+      <c r="E12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="25" t="s">
+      <c r="K12" s="19" t="s">
         <v>40</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="25" t="s">
+      <c r="M12" s="19" t="s">
         <v>46</v>
       </c>
       <c r="N12" s="4"/>

</xml_diff>

<commit_message>
Update crop_classification tables and column_name_translation tabels
</commit_message>
<xml_diff>
--- a/tables/column_name_translations/AT_column_name_translation.xlsx
+++ b/tables/column_name_translations/AT_column_name_translation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BC61BA-3EBD-4661-81F1-5514CEABA980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC853EED-90BA-49C6-AC42-33CDC05C786D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
   <si>
     <t>field_id</t>
   </si>
@@ -219,11 +219,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -524,7 +530,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+      <selection pane="topRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,31 +592,31 @@
       <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="25" t="s">
         <v>47</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -636,9 +642,15 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>37</v>
       </c>
@@ -673,31 +685,31 @@
       <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="H4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>38</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="25" t="s">
         <v>43</v>
       </c>
       <c r="N4" s="4"/>
@@ -717,34 +729,34 @@
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="E5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="F5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="G5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="H5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="20" t="s">
         <v>39</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="25" t="s">
         <v>44</v>
       </c>
       <c r="N5" s="4"/>
@@ -882,25 +894,31 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19" t="s">
+      <c r="E11" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="F11" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="G11" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="H11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>14</v>
       </c>
       <c r="L11" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="19"/>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -912,34 +930,28 @@
       <c r="C12" s="4">
         <v>1</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="16" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="K12" s="19" t="s">
+      <c r="K12" s="25" t="s">
         <v>40</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="25" t="s">
         <v>46</v>
       </c>
       <c r="N12" s="4"/>

</xml_diff>